<commit_message>
Fix the DaPaiWei deceased date issue pointed out by Brother Guo and Sister Chan.  - Format check  - Valid date range check
</commit_message>
<xml_diff>
--- a/PaiWei/Templates/pwTemplate.xlsx
+++ b/PaiWei/Templates/pwTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berttan/MacPLC/admin/PaiWei/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85265741-3AFD-E34B-A56F-501B64428D43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181E50C3-F4BB-5645-ADA9-6875BC3919EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="祈福消災" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="12個月內往生親友牌位" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="W001A" localSheetId="5">'12個月內往生親友牌位'!$B$3:$F$519</definedName>
+    <definedName name="W001A" localSheetId="5">'12個月內往生親友牌位'!$B$3:$F$522</definedName>
     <definedName name="W001A" localSheetId="3">往生親友牌位!$B$3:$E$519</definedName>
   </definedNames>
   <calcPr calcId="150000"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>D_Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -304,6 +304,30 @@
   </si>
   <si>
     <t>朋友</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCCC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MMMM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZZZZ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UUUU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VVVV</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3413,13 +3437,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>550336</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>152398</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1600203</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>93131</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3578,13 +3602,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>143928</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>135466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1193796</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>101597</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3753,13 +3777,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>93126</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>152398</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1142993</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>93131</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3928,13 +3952,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>101601</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>135466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1151468</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>101597</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4103,13 +4127,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>135466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1735667</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>101597</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4592,7 +4616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -4806,10 +4830,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C93509-993E-BD47-ABFA-94FF3412B35C}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -4873,20 +4897,71 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="10">
+        <v>43282</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C5" s="10">
         <v>43309</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="10">
+        <v>43524</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="10">
+        <v>43373</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feature:	User Guide in Chinese Files: 	PaiWei.js 	Templates/pwTemplate.xlsx 	UG.php 	img/allImgXLS.png 	img/editDaPaiWei.png 	img/inputXLS.png 	img/newDaPaiWei.png 	img/pwMain.png 	img/saveActive.png 	img/saveAsCSV.png 	img/saveAsSel.png 	img/saveChgDaPaiWei.png 	img/upldBox.png 	img/upldFile.png 	img/upldPaiWei.png 	index.php 	upldPaiWeiForm.php
</commit_message>
<xml_diff>
--- a/PaiWei/Templates/pwTemplate.xlsx
+++ b/PaiWei/Templates/pwTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berttan/MacPLC/admin/PaiWei/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berttan/temp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181E50C3-F4BB-5645-ADA9-6875BC3919EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1939EA89-58A6-FF4F-9709-50588AF41414}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="560" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="祈福消災" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="W001A" localSheetId="5">'12個月內往生親友牌位'!$B$3:$F$522</definedName>
     <definedName name="W001A" localSheetId="3">往生親友牌位!$B$3:$E$519</definedName>
   </definedNames>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>D_Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,10 +213,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>朋有</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AAAA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -248,10 +244,6 @@
   </si>
   <si>
     <t>deceasedDate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>佛光祝照受益者姓名        Well-blessing Recipient's Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -330,6 +322,10 @@
     <t>VVVV</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>祈福消災受益者姓名        Well-blessing Recipient's Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -338,7 +334,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -417,12 +413,6 @@
       <charset val="136"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Heiti TC Light"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -433,7 +423,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Heiti TC Light"/>
-      <charset val="136"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -575,44 +565,58 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -679,6 +683,9 @@
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -1034,6 +1041,9 @@
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -1523,15 +1533,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>338669</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>169334</xdr:rowOff>
+      <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1049867</xdr:colOff>
+      <xdr:colOff>1388536</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>160867</xdr:rowOff>
+      <xdr:rowOff>118532</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1546,7 +1556,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="880534"/>
+          <a:off x="338669" y="1540932"/>
           <a:ext cx="1049867" cy="2048933"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
@@ -1678,7 +1688,7 @@
               <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
               <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>只要祖先姓式</a:t>
+            <a:t>只要祖先姓氏</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1882,6 +1892,9 @@
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -2541,17 +2554,7 @@
               <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
               <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>您的或啟請者的全名及關</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" b="1">
-              <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
-              <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
-            </a:rPr>
-            <a:t>係</a:t>
+            <a:t>您的或啟請者的全名</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2945,6 +2948,9 @@
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3261,22 +3267,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>118533</xdr:colOff>
+      <xdr:colOff>55040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>67733</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>318485</xdr:colOff>
+      <xdr:colOff>254992</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>338667</xdr:rowOff>
+      <xdr:rowOff>313267</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Left Arrow 1">
+        <xdr:cNvPr id="8" name="Left Arrow 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8B67332-00CC-FD40-93C6-70F1480C5B89}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B5F8889-CBE5-B545-8167-C33FEF6F41C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3284,12 +3290,15 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6341533" y="67733"/>
-          <a:ext cx="2358952" cy="651934"/>
+          <a:off x="8538640" y="38100"/>
+          <a:ext cx="2358952" cy="1075267"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -3436,22 +3445,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>550336</xdr:colOff>
+      <xdr:colOff>472021</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>152398</xdr:rowOff>
+      <xdr:rowOff>80434</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1600203</xdr:colOff>
+      <xdr:colOff>1521888</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>93131</xdr:rowOff>
+      <xdr:rowOff>71967</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Up Arrow 2">
+        <xdr:cNvPr id="9" name="Up Arrow 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3790BBBD-0CF3-9649-8717-FBE3F509FED5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC67D167-9BD4-D344-9860-1EA3C9E8F7DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3459,8 +3468,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1769536" y="1371598"/>
-          <a:ext cx="1049867" cy="2683933"/>
+          <a:off x="1691221" y="2404534"/>
+          <a:ext cx="1049867" cy="2734733"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
           <a:avLst/>
@@ -3591,7 +3600,17 @@
               <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
               <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>往生者全名</a:t>
+            <a:t>往生者全名及關</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
+              <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
+            </a:rPr>
+            <a:t>係</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3601,22 +3620,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>143928</xdr:colOff>
+      <xdr:colOff>143936</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>135466</xdr:rowOff>
+      <xdr:rowOff>50802</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1193796</xdr:colOff>
+      <xdr:colOff>1210737</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>101597</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Up Arrow 3">
+        <xdr:cNvPr id="10" name="Up Arrow 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23C23E48-FEC3-BD4C-8783-2B5E4F310F63}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB13FA36-2155-D140-ACC4-0FB8EBBFF37D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3624,8 +3643,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8483595" y="1354666"/>
-          <a:ext cx="1049868" cy="3852331"/>
+          <a:off x="7294036" y="2374902"/>
+          <a:ext cx="1066801" cy="3924298"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
           <a:avLst/>
@@ -3756,17 +3775,7 @@
               <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
               <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>您的或啟請者的全名及關</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" b="1">
-              <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
-              <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
-            </a:rPr>
-            <a:t>係</a:t>
+            <a:t>您的或啟請者的全名</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3776,22 +3785,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>93126</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>152398</xdr:rowOff>
+      <xdr:rowOff>80433</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1142993</xdr:colOff>
+      <xdr:colOff>1049867</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>93131</xdr:rowOff>
+      <xdr:rowOff>71966</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Up Arrow 4">
+        <xdr:cNvPr id="11" name="Up Arrow 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF22B317-725A-5A44-85BF-A267903EA309}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85250EC2-6D40-D74C-B685-E1DF51C86C6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3799,8 +3808,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="93126" y="1371598"/>
-          <a:ext cx="1049867" cy="2683933"/>
+          <a:off x="0" y="2404533"/>
+          <a:ext cx="1049867" cy="2734733"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
           <a:avLst/>
@@ -3951,22 +3960,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>101601</xdr:colOff>
+      <xdr:colOff>91025</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>135466</xdr:rowOff>
+      <xdr:rowOff>46568</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1151468</xdr:colOff>
+      <xdr:colOff>1140892</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>101597</xdr:rowOff>
+      <xdr:rowOff>84666</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Up Arrow 5">
+        <xdr:cNvPr id="12" name="Up Arrow 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43772F6F-B4D0-2A41-8ABA-3DA86A099584}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03F1F714-13CC-2D40-BDF8-583DAB0459C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3974,8 +3983,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4436534" y="1354666"/>
-          <a:ext cx="1049867" cy="3852331"/>
+          <a:off x="6021925" y="2370668"/>
+          <a:ext cx="1049867" cy="3924298"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
           <a:avLst/>
@@ -4126,22 +4135,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:colOff>700625</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>135466</xdr:rowOff>
+      <xdr:rowOff>46568</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1735667</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>101597</xdr:rowOff>
+      <xdr:colOff>1750492</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Up Arrow 6">
+        <xdr:cNvPr id="13" name="Up Arrow 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BE4F9CC-063C-7649-9CA7-AA0EFAEA6464}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{104EF709-A85C-904C-A4DF-759BE643CD4F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4149,8 +4158,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5020733" y="1354666"/>
-          <a:ext cx="1049867" cy="3852331"/>
+          <a:off x="4231225" y="2370668"/>
+          <a:ext cx="1049867" cy="2302932"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
           <a:avLst/>
@@ -4277,12 +4286,16 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" b="1">
+            <a:rPr lang="zh-TW" altLang="en-US" b="1">
               <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
               <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>一年之內的往生年月日</a:t>
+            <a:t>往生者往生日期</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" b="1">
+            <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
+            <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4564,47 +4577,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="28.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="42">
-      <c r="A1" s="12" t="s">
-        <v>27</v>
+      <c r="A1" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="19" thickBot="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1" selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4616,42 +4631,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="45.625" customWidth="1"/>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="42">
-      <c r="A1" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>29</v>
+      <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19" thickBot="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>25</v>
+      <c r="B3" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1" selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4662,42 +4679,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="10.625" customWidth="1"/>
-    <col min="2" max="2" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="63">
-      <c r="A1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>35</v>
+      <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" thickBot="1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1" selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4708,84 +4727,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="63">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="A4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1" selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4796,32 +4817,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
+    <col min="1" max="1" width="25.625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="42">
-      <c r="A1" s="14" t="s">
-        <v>36</v>
+      <c r="A1" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="30" customHeight="1" thickBot="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1" selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4832,139 +4855,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0C93509-993E-BD47-ABFA-94FF3412B35C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="63">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>34</v>
+      <c r="D1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" thickBot="1">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="14">
         <v>43251</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="14">
+        <v>43282</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" s="10">
-        <v>43282</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="C5" s="14">
         <v>43309</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="10">
+      <c r="A6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="14">
         <v>43524</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
+      <c r="D6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="10">
+      <c r="A7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="14">
         <v>43373</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
+      <c r="D7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" scenarios="1" selectLockedCells="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Feature:	User Guide in English Files: 	PaiWei/Templates/e_pwTemplate.xlsx 	PaiWei/Templates/pwTemplate.xlsx 	PaiWei/UG.php 	PaiWei/img/.gitignore 	PaiWei/img/e_allImgXLS.png 	PaiWei/img/e_editDaPaiWei.png 	PaiWei/img/e_inputXLS.png 	PaiWei/img/e_newDaPaiWei.png 	PaiWei/img/epwMain.png -> ../img/e_pwMain.png 	PaiWei/img/e_saveChgDaPaiWei.png 	PaiWei/img/e_upldBox.png 	PaiWei/img/e_upldFile.png 	PaiWei/img/e_upldPaiWei.png
</commit_message>
<xml_diff>
--- a/PaiWei/Templates/pwTemplate.xlsx
+++ b/PaiWei/Templates/pwTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berttan/temp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berttan/MacPLC/admin/PaiWei/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1939EA89-58A6-FF4F-9709-50588AF41414}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4249FC-F33F-7A4E-BBC7-36D5AD4AD493}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2231,8 +2231,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1617131</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>135467</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2247,8 +2247,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1786464" y="1642534"/>
-          <a:ext cx="1049867" cy="2683933"/>
+          <a:off x="1784347" y="2078567"/>
+          <a:ext cx="1049867" cy="1921933"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
           <a:avLst/>
@@ -2379,17 +2379,7 @@
               <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
               <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>往生者全名及關</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" b="1">
-              <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
-              <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
-            </a:rPr>
-            <a:t>係</a:t>
+            <a:t>往生者全名</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3447,13 +3437,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>472021</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>80434</xdr:rowOff>
+      <xdr:rowOff>80435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1521888</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>71967</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3468,8 +3458,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1691221" y="2404534"/>
-          <a:ext cx="1049867" cy="2734733"/>
+          <a:off x="1691221" y="2404535"/>
+          <a:ext cx="1049867" cy="1748366"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
           <a:avLst/>
@@ -3600,17 +3590,7 @@
               <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
               <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
             </a:rPr>
-            <a:t>往生者全名及關</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" b="1">
-              <a:latin typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
-              <a:ea typeface="TSC UKai M TT" panose="02010609030101010101" pitchFamily="49" charset="-122"/>
-            </a:rPr>
-            <a:t>係</a:t>
+            <a:t>往生者全名</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>

</xml_diff>